<commit_message>
Updated A Funct with graph labels
</commit_message>
<xml_diff>
--- a/A_funct.xlsx
+++ b/A_funct.xlsx
@@ -428,21 +428,45 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="235715200"/>
-        <c:axId val="235757952"/>
+        <c:axId val="212315136"/>
+        <c:axId val="212316928"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="235715200"/>
+        <c:axId val="212315136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Distance</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> From Sensors (in)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235757952"/>
+        <c:crossAx val="212316928"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -450,18 +474,37 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="235757952"/>
+        <c:axId val="212316928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Voltage</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="235715200"/>
+        <c:crossAx val="212315136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -807,8 +850,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="Q23" sqref="Q23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +952,7 @@
         <v>0.29399999999999998</v>
       </c>
       <c r="C3" s="1">
-        <f t="shared" ref="C3:C13" si="0">(B3)*1023</f>
+        <f t="shared" ref="C3:C12" si="0">(B3)*1023</f>
         <v>300.762</v>
       </c>
       <c r="D3" s="1" t="str">

</xml_diff>